<commit_message>
Update NHS England deaths data (accessed 22 July 2020)
</commit_message>
<xml_diff>
--- a/Data/NHS England data/coronavirus-deaths_latest.xlsx
+++ b/Data/NHS England data/coronavirus-deaths_latest.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://leeds365-my.sharepoint.com/personal/medkarn_leeds_ac_uk/Documents/Postdoc - Urban Analytics (LIDA)/Research/Covid exponential growth/Data/NHS England data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://leeds365-my.sharepoint.com/personal/medkarn_leeds_ac_uk/Documents/Postdoc - Urban Analytics (LIDA)/Research/COVID-19/Counterfactual growth (England)/covid-counterfactual/Data/NHS England data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="8_{101EDDEF-0E45-A041-80AC-552520C86941}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{20A44B26-A2BD-D94E-8CAD-F7FAA74F845F}"/>
+  <xr:revisionPtr revIDLastSave="14" documentId="8_{101EDDEF-0E45-A041-80AC-552520C86941}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{F10053C4-811B-544A-9E5D-FEEFAD6284DF}"/>
   <bookViews>
-    <workbookView xWindow="5200" yWindow="3640" windowWidth="28440" windowHeight="15900" xr2:uid="{FA57FF27-1EE2-9C45-AAFC-CC52811345F8}"/>
+    <workbookView xWindow="4080" yWindow="4140" windowWidth="28440" windowHeight="15900" xr2:uid="{FA57FF27-1EE2-9C45-AAFC-CC52811345F8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="5">
   <si>
     <t>Area name</t>
   </si>
@@ -417,10 +417,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46E7D4FB-2BB9-244A-B945-F1EC7D3119F1}">
-  <dimension ref="A1:D98"/>
+  <dimension ref="A1:D143"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:H1048576"/>
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -540,11 +540,11 @@
         <v>43897</v>
       </c>
       <c r="C8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D8">
         <f>SUM($C$2:C8)</f>
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -555,11 +555,11 @@
         <v>43898</v>
       </c>
       <c r="C9">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D9">
         <f>SUM($C$2:C9)</f>
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -574,7 +574,7 @@
       </c>
       <c r="D10">
         <f>SUM($C$2:C10)</f>
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -589,7 +589,7 @@
       </c>
       <c r="D11">
         <f>SUM($C$2:C11)</f>
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -600,11 +600,11 @@
         <v>43901</v>
       </c>
       <c r="C12">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D12">
         <f>SUM($C$2:C12)</f>
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -619,7 +619,7 @@
       </c>
       <c r="D13">
         <f>SUM($C$2:C13)</f>
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -634,7 +634,7 @@
       </c>
       <c r="D14">
         <f>SUM($C$2:C14)</f>
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -645,11 +645,11 @@
         <v>43904</v>
       </c>
       <c r="C15">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D15">
         <f>SUM($C$2:C15)</f>
-        <v>86</v>
+        <v>81</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -660,11 +660,11 @@
         <v>43905</v>
       </c>
       <c r="C16">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D16">
         <f>SUM($C$2:C16)</f>
-        <v>114</v>
+        <v>108</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
@@ -675,11 +675,11 @@
         <v>43906</v>
       </c>
       <c r="C17">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D17">
         <f>SUM($C$2:C17)</f>
-        <v>156</v>
+        <v>148</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
@@ -690,11 +690,11 @@
         <v>43907</v>
       </c>
       <c r="C18">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D18">
         <f>SUM($C$2:C18)</f>
-        <v>204</v>
+        <v>194</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
@@ -705,11 +705,11 @@
         <v>43908</v>
       </c>
       <c r="C19">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="D19">
         <f>SUM($C$2:C19)</f>
-        <v>273</v>
+        <v>259</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
@@ -720,11 +720,11 @@
         <v>43909</v>
       </c>
       <c r="C20">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D20">
         <f>SUM($C$2:C20)</f>
-        <v>337</v>
+        <v>322</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
@@ -735,11 +735,11 @@
         <v>43910</v>
       </c>
       <c r="C21">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D21">
         <f>SUM($C$2:C21)</f>
-        <v>444</v>
+        <v>427</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
@@ -750,11 +750,11 @@
         <v>43911</v>
       </c>
       <c r="C22">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D22">
         <f>SUM($C$2:C22)</f>
-        <v>548</v>
+        <v>530</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
@@ -765,11 +765,11 @@
         <v>43912</v>
       </c>
       <c r="C23">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D23">
         <f>SUM($C$2:C23)</f>
-        <v>699</v>
+        <v>679</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
@@ -780,11 +780,11 @@
         <v>43913</v>
       </c>
       <c r="C24">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="D24">
         <f>SUM($C$2:C24)</f>
-        <v>861</v>
+        <v>838</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
@@ -795,11 +795,11 @@
         <v>43914</v>
       </c>
       <c r="C25">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D25">
         <f>SUM($C$2:C25)</f>
-        <v>1066</v>
+        <v>1042</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
@@ -810,11 +810,11 @@
         <v>43915</v>
       </c>
       <c r="C26">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D26">
         <f>SUM($C$2:C26)</f>
-        <v>1330</v>
+        <v>1305</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
@@ -829,7 +829,7 @@
       </c>
       <c r="D27">
         <f>SUM($C$2:C27)</f>
-        <v>1655</v>
+        <v>1630</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
@@ -844,7 +844,7 @@
       </c>
       <c r="D28">
         <f>SUM($C$2:C28)</f>
-        <v>2005</v>
+        <v>1980</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
@@ -859,7 +859,7 @@
       </c>
       <c r="D29">
         <f>SUM($C$2:C29)</f>
-        <v>2364</v>
+        <v>2339</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
@@ -870,11 +870,11 @@
         <v>43919</v>
       </c>
       <c r="C30">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="D30">
         <f>SUM($C$2:C30)</f>
-        <v>2802</v>
+        <v>2776</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
@@ -885,11 +885,11 @@
         <v>43920</v>
       </c>
       <c r="C31">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="D31">
         <f>SUM($C$2:C31)</f>
-        <v>3299</v>
+        <v>3272</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
@@ -904,7 +904,7 @@
       </c>
       <c r="D32">
         <f>SUM($C$2:C32)</f>
-        <v>3873</v>
+        <v>3846</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
@@ -915,11 +915,11 @@
         <v>43922</v>
       </c>
       <c r="C33">
-        <v>643</v>
+        <v>644</v>
       </c>
       <c r="D33">
         <f>SUM($C$2:C33)</f>
-        <v>4516</v>
+        <v>4490</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
@@ -930,11 +930,11 @@
         <v>43923</v>
       </c>
       <c r="C34">
-        <v>644</v>
+        <v>647</v>
       </c>
       <c r="D34">
         <f>SUM($C$2:C34)</f>
-        <v>5160</v>
+        <v>5137</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
@@ -949,7 +949,7 @@
       </c>
       <c r="D35">
         <f>SUM($C$2:C35)</f>
-        <v>5857</v>
+        <v>5834</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
@@ -964,7 +964,7 @@
       </c>
       <c r="D36">
         <f>SUM($C$2:C36)</f>
-        <v>6634</v>
+        <v>6611</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
@@ -979,7 +979,7 @@
       </c>
       <c r="D37">
         <f>SUM($C$2:C37)</f>
-        <v>7377</v>
+        <v>7354</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
@@ -990,11 +990,11 @@
         <v>43927</v>
       </c>
       <c r="C38">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="D38">
         <f>SUM($C$2:C38)</f>
-        <v>8104</v>
+        <v>8080</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
@@ -1005,11 +1005,11 @@
         <v>43928</v>
       </c>
       <c r="C39">
-        <v>809</v>
+        <v>812</v>
       </c>
       <c r="D39">
         <f>SUM($C$2:C39)</f>
-        <v>8913</v>
+        <v>8892</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
@@ -1024,7 +1024,7 @@
       </c>
       <c r="D40">
         <f>SUM($C$2:C40)</f>
-        <v>9812</v>
+        <v>9791</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
@@ -1035,11 +1035,11 @@
         <v>43930</v>
       </c>
       <c r="C41">
-        <v>789</v>
+        <v>790</v>
       </c>
       <c r="D41">
         <f>SUM($C$2:C41)</f>
-        <v>10601</v>
+        <v>10581</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
@@ -1054,7 +1054,7 @@
       </c>
       <c r="D42">
         <f>SUM($C$2:C42)</f>
-        <v>11340</v>
+        <v>11320</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
@@ -1065,11 +1065,11 @@
         <v>43932</v>
       </c>
       <c r="C43">
-        <v>776</v>
+        <v>779</v>
       </c>
       <c r="D43">
         <f>SUM($C$2:C43)</f>
-        <v>12116</v>
+        <v>12099</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
@@ -1080,11 +1080,11 @@
         <v>43933</v>
       </c>
       <c r="C44">
-        <v>719</v>
+        <v>717</v>
       </c>
       <c r="D44">
         <f>SUM($C$2:C44)</f>
-        <v>12835</v>
+        <v>12816</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
@@ -1095,11 +1095,11 @@
         <v>43934</v>
       </c>
       <c r="C45">
-        <v>696</v>
+        <v>698</v>
       </c>
       <c r="D45">
         <f>SUM($C$2:C45)</f>
-        <v>13531</v>
+        <v>13514</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
@@ -1114,7 +1114,7 @@
       </c>
       <c r="D46">
         <f>SUM($C$2:C46)</f>
-        <v>14178</v>
+        <v>14161</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
@@ -1129,7 +1129,7 @@
       </c>
       <c r="D47">
         <f>SUM($C$2:C47)</f>
-        <v>14863</v>
+        <v>14846</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
@@ -1140,11 +1140,11 @@
         <v>43937</v>
       </c>
       <c r="C48">
-        <v>637</v>
+        <v>639</v>
       </c>
       <c r="D48">
         <f>SUM($C$2:C48)</f>
-        <v>15500</v>
+        <v>15485</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
@@ -1155,11 +1155,11 @@
         <v>43938</v>
       </c>
       <c r="C49">
-        <v>607</v>
+        <v>609</v>
       </c>
       <c r="D49">
         <f>SUM($C$2:C49)</f>
-        <v>16107</v>
+        <v>16094</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
@@ -1174,7 +1174,7 @@
       </c>
       <c r="D50">
         <f>SUM($C$2:C50)</f>
-        <v>16677</v>
+        <v>16664</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
@@ -1185,11 +1185,11 @@
         <v>43940</v>
       </c>
       <c r="C51">
-        <v>521</v>
+        <v>522</v>
       </c>
       <c r="D51">
         <f>SUM($C$2:C51)</f>
-        <v>17198</v>
+        <v>17186</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
@@ -1200,11 +1200,11 @@
         <v>43941</v>
       </c>
       <c r="C52">
-        <v>563</v>
+        <v>565</v>
       </c>
       <c r="D52">
         <f>SUM($C$2:C52)</f>
-        <v>17761</v>
+        <v>17751</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
@@ -1219,7 +1219,7 @@
       </c>
       <c r="D53">
         <f>SUM($C$2:C53)</f>
-        <v>18245</v>
+        <v>18235</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
@@ -1230,11 +1230,11 @@
         <v>43943</v>
       </c>
       <c r="C54">
-        <v>499</v>
+        <v>501</v>
       </c>
       <c r="D54">
         <f>SUM($C$2:C54)</f>
-        <v>18744</v>
+        <v>18736</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
@@ -1245,11 +1245,11 @@
         <v>43944</v>
       </c>
       <c r="C55">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="D55">
         <f>SUM($C$2:C55)</f>
-        <v>19194</v>
+        <v>19187</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
@@ -1264,7 +1264,7 @@
       </c>
       <c r="D56">
         <f>SUM($C$2:C56)</f>
-        <v>19631</v>
+        <v>19624</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
@@ -1275,11 +1275,11 @@
         <v>43946</v>
       </c>
       <c r="C57">
-        <v>383</v>
+        <v>385</v>
       </c>
       <c r="D57">
         <f>SUM($C$2:C57)</f>
-        <v>20014</v>
+        <v>20009</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
@@ -1294,7 +1294,7 @@
       </c>
       <c r="D58">
         <f>SUM($C$2:C58)</f>
-        <v>20394</v>
+        <v>20389</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
@@ -1305,11 +1305,11 @@
         <v>43948</v>
       </c>
       <c r="C59">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="D59">
         <f>SUM($C$2:C59)</f>
-        <v>20737</v>
+        <v>20733</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
@@ -1320,11 +1320,11 @@
         <v>43949</v>
       </c>
       <c r="C60">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="D60">
         <f>SUM($C$2:C60)</f>
-        <v>21077</v>
+        <v>21074</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
@@ -1335,11 +1335,11 @@
         <v>43950</v>
       </c>
       <c r="C61">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="D61">
         <f>SUM($C$2:C61)</f>
-        <v>21399</v>
+        <v>21398</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
@@ -1350,11 +1350,11 @@
         <v>43951</v>
       </c>
       <c r="C62">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="D62">
         <f>SUM($C$2:C62)</f>
-        <v>21709</v>
+        <v>21710</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
@@ -1365,11 +1365,11 @@
         <v>43952</v>
       </c>
       <c r="C63">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="D63">
         <f>SUM($C$2:C63)</f>
-        <v>22014</v>
+        <v>22016</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
@@ -1380,11 +1380,11 @@
         <v>43953</v>
       </c>
       <c r="C64">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="D64">
         <f>SUM($C$2:C64)</f>
-        <v>22281</v>
+        <v>22284</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
@@ -1399,7 +1399,7 @@
       </c>
       <c r="D65">
         <f>SUM($C$2:C65)</f>
-        <v>22532</v>
+        <v>22535</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
@@ -1410,11 +1410,11 @@
         <v>43955</v>
       </c>
       <c r="C66">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="D66">
         <f>SUM($C$2:C66)</f>
-        <v>22789</v>
+        <v>22794</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
@@ -1425,11 +1425,11 @@
         <v>43956</v>
       </c>
       <c r="C67">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="D67">
         <f>SUM($C$2:C67)</f>
-        <v>23038</v>
+        <v>23045</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
@@ -1440,11 +1440,11 @@
         <v>43957</v>
       </c>
       <c r="C68">
-        <v>262</v>
+        <v>266</v>
       </c>
       <c r="D68">
         <f>SUM($C$2:C68)</f>
-        <v>23300</v>
+        <v>23311</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
@@ -1459,7 +1459,7 @@
       </c>
       <c r="D69">
         <f>SUM($C$2:C69)</f>
-        <v>23555</v>
+        <v>23566</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
@@ -1470,11 +1470,11 @@
         <v>43959</v>
       </c>
       <c r="C70">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="D70">
         <f>SUM($C$2:C70)</f>
-        <v>23767</v>
+        <v>23779</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
@@ -1485,11 +1485,11 @@
         <v>43960</v>
       </c>
       <c r="C71">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="D71">
         <f>SUM($C$2:C71)</f>
-        <v>23969</v>
+        <v>23982</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
@@ -1500,11 +1500,11 @@
         <v>43961</v>
       </c>
       <c r="C72">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="D72">
         <f>SUM($C$2:C72)</f>
-        <v>24163</v>
+        <v>24178</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
@@ -1515,11 +1515,11 @@
         <v>43962</v>
       </c>
       <c r="C73">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="D73">
         <f>SUM($C$2:C73)</f>
-        <v>24328</v>
+        <v>24344</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
@@ -1534,7 +1534,7 @@
       </c>
       <c r="D74">
         <f>SUM($C$2:C74)</f>
-        <v>24511</v>
+        <v>24527</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
@@ -1545,11 +1545,11 @@
         <v>43964</v>
       </c>
       <c r="C75">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="D75">
         <f>SUM($C$2:C75)</f>
-        <v>24670</v>
+        <v>24689</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
@@ -1560,11 +1560,11 @@
         <v>43965</v>
       </c>
       <c r="C76">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="D76">
         <f>SUM($C$2:C76)</f>
-        <v>24846</v>
+        <v>24868</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
@@ -1575,11 +1575,11 @@
         <v>43966</v>
       </c>
       <c r="C77">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="D77">
         <f>SUM($C$2:C77)</f>
-        <v>25016</v>
+        <v>25039</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
@@ -1594,7 +1594,7 @@
       </c>
       <c r="D78">
         <f>SUM($C$2:C78)</f>
-        <v>25183</v>
+        <v>25206</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
@@ -1605,11 +1605,11 @@
         <v>43968</v>
       </c>
       <c r="C79">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D79">
         <f>SUM($C$2:C79)</f>
-        <v>25319</v>
+        <v>25343</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
@@ -1620,11 +1620,11 @@
         <v>43969</v>
       </c>
       <c r="C80">
-        <v>152</v>
+        <v>158</v>
       </c>
       <c r="D80">
         <f>SUM($C$2:C80)</f>
-        <v>25471</v>
+        <v>25501</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.2">
@@ -1635,11 +1635,11 @@
         <v>43970</v>
       </c>
       <c r="C81">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="D81">
         <f>SUM($C$2:C81)</f>
-        <v>25612</v>
+        <v>25645</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.2">
@@ -1650,11 +1650,11 @@
         <v>43971</v>
       </c>
       <c r="C82">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="D82">
         <f>SUM($C$2:C82)</f>
-        <v>25762</v>
+        <v>25798</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.2">
@@ -1665,11 +1665,11 @@
         <v>43972</v>
       </c>
       <c r="C83">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="D83">
         <f>SUM($C$2:C83)</f>
-        <v>25908</v>
+        <v>25947</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.2">
@@ -1680,11 +1680,11 @@
         <v>43973</v>
       </c>
       <c r="C84">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D84">
         <f>SUM($C$2:C84)</f>
-        <v>26028</v>
+        <v>26068</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.2">
@@ -1695,11 +1695,11 @@
         <v>43974</v>
       </c>
       <c r="C85">
-        <v>122</v>
+        <v>128</v>
       </c>
       <c r="D85">
         <f>SUM($C$2:C85)</f>
-        <v>26150</v>
+        <v>26196</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.2">
@@ -1710,11 +1710,11 @@
         <v>43975</v>
       </c>
       <c r="C86">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="D86">
         <f>SUM($C$2:C86)</f>
-        <v>26260</v>
+        <v>26312</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.2">
@@ -1725,11 +1725,11 @@
         <v>43976</v>
       </c>
       <c r="C87">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="D87">
         <f>SUM($C$2:C87)</f>
-        <v>26389</v>
+        <v>26445</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.2">
@@ -1740,11 +1740,11 @@
         <v>43977</v>
       </c>
       <c r="C88">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="D88">
         <f>SUM($C$2:C88)</f>
-        <v>26522</v>
+        <v>26583</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.2">
@@ -1755,11 +1755,11 @@
         <v>43978</v>
       </c>
       <c r="C89">
-        <v>114</v>
+        <v>120</v>
       </c>
       <c r="D89">
         <f>SUM($C$2:C89)</f>
-        <v>26636</v>
+        <v>26703</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.2">
@@ -1770,11 +1770,11 @@
         <v>43979</v>
       </c>
       <c r="C90">
-        <v>116</v>
+        <v>124</v>
       </c>
       <c r="D90">
         <f>SUM($C$2:C90)</f>
-        <v>26752</v>
+        <v>26827</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.2">
@@ -1785,11 +1785,11 @@
         <v>43980</v>
       </c>
       <c r="C91">
-        <v>106</v>
+        <v>116</v>
       </c>
       <c r="D91">
         <f>SUM($C$2:C91)</f>
-        <v>26858</v>
+        <v>26943</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.2">
@@ -1800,11 +1800,11 @@
         <v>43981</v>
       </c>
       <c r="C92">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="D92">
         <f>SUM($C$2:C92)</f>
-        <v>26945</v>
+        <v>27035</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.2">
@@ -1815,11 +1815,11 @@
         <v>43982</v>
       </c>
       <c r="C93">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="D93">
         <f>SUM($C$2:C93)</f>
-        <v>27022</v>
+        <v>27118</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.2">
@@ -1830,11 +1830,11 @@
         <v>43983</v>
       </c>
       <c r="C94">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="D94">
         <f>SUM($C$2:C94)</f>
-        <v>27107</v>
+        <v>27212</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.2">
@@ -1845,11 +1845,11 @@
         <v>43984</v>
       </c>
       <c r="C95">
-        <v>96</v>
+        <v>109</v>
       </c>
       <c r="D95">
         <f>SUM($C$2:C95)</f>
-        <v>27203</v>
+        <v>27321</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.2">
@@ -1860,11 +1860,11 @@
         <v>43985</v>
       </c>
       <c r="C96">
-        <v>85</v>
+        <v>110</v>
       </c>
       <c r="D96">
         <f>SUM($C$2:C96)</f>
-        <v>27288</v>
+        <v>27431</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.2">
@@ -1875,11 +1875,11 @@
         <v>43986</v>
       </c>
       <c r="C97">
-        <v>53</v>
+        <v>83</v>
       </c>
       <c r="D97">
         <f>SUM($C$2:C97)</f>
-        <v>27341</v>
+        <v>27514</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.2">
@@ -1890,11 +1890,686 @@
         <v>43987</v>
       </c>
       <c r="C98">
-        <v>17</v>
+        <v>86</v>
       </c>
       <c r="D98">
         <f>SUM($C$2:C98)</f>
-        <v>27358</v>
+        <v>27600</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A99" t="s">
+        <v>4</v>
+      </c>
+      <c r="B99" s="1">
+        <v>43988</v>
+      </c>
+      <c r="C99">
+        <v>83</v>
+      </c>
+      <c r="D99">
+        <f>SUM($C$2:C99)</f>
+        <v>27683</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A100" t="s">
+        <v>4</v>
+      </c>
+      <c r="B100" s="1">
+        <v>43989</v>
+      </c>
+      <c r="C100">
+        <v>80</v>
+      </c>
+      <c r="D100">
+        <f>SUM($C$2:C100)</f>
+        <v>27763</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A101" t="s">
+        <v>4</v>
+      </c>
+      <c r="B101" s="1">
+        <v>43990</v>
+      </c>
+      <c r="C101">
+        <v>73</v>
+      </c>
+      <c r="D101">
+        <f>SUM($C$2:C101)</f>
+        <v>27836</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A102" t="s">
+        <v>4</v>
+      </c>
+      <c r="B102" s="1">
+        <v>43991</v>
+      </c>
+      <c r="C102">
+        <v>67</v>
+      </c>
+      <c r="D102">
+        <f>SUM($C$2:C102)</f>
+        <v>27903</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A103" t="s">
+        <v>4</v>
+      </c>
+      <c r="B103" s="1">
+        <v>43992</v>
+      </c>
+      <c r="C103">
+        <v>77</v>
+      </c>
+      <c r="D103">
+        <f>SUM($C$2:C103)</f>
+        <v>27980</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A104" t="s">
+        <v>4</v>
+      </c>
+      <c r="B104" s="1">
+        <v>43993</v>
+      </c>
+      <c r="C104">
+        <v>49</v>
+      </c>
+      <c r="D104">
+        <f>SUM($C$2:C104)</f>
+        <v>28029</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A105" t="s">
+        <v>4</v>
+      </c>
+      <c r="B105" s="1">
+        <v>43994</v>
+      </c>
+      <c r="C105">
+        <v>52</v>
+      </c>
+      <c r="D105">
+        <f>SUM($C$2:C105)</f>
+        <v>28081</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A106" t="s">
+        <v>4</v>
+      </c>
+      <c r="B106" s="1">
+        <v>43995</v>
+      </c>
+      <c r="C106">
+        <v>43</v>
+      </c>
+      <c r="D106">
+        <f>SUM($C$2:C106)</f>
+        <v>28124</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A107" t="s">
+        <v>4</v>
+      </c>
+      <c r="B107" s="1">
+        <v>43996</v>
+      </c>
+      <c r="C107">
+        <v>58</v>
+      </c>
+      <c r="D107">
+        <f>SUM($C$2:C107)</f>
+        <v>28182</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A108" t="s">
+        <v>4</v>
+      </c>
+      <c r="B108" s="1">
+        <v>43997</v>
+      </c>
+      <c r="C108">
+        <v>56</v>
+      </c>
+      <c r="D108">
+        <f>SUM($C$2:C108)</f>
+        <v>28238</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A109" t="s">
+        <v>4</v>
+      </c>
+      <c r="B109" s="1">
+        <v>43998</v>
+      </c>
+      <c r="C109">
+        <v>60</v>
+      </c>
+      <c r="D109">
+        <f>SUM($C$2:C109)</f>
+        <v>28298</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A110" t="s">
+        <v>4</v>
+      </c>
+      <c r="B110" s="1">
+        <v>43999</v>
+      </c>
+      <c r="C110">
+        <v>50</v>
+      </c>
+      <c r="D110">
+        <f>SUM($C$2:C110)</f>
+        <v>28348</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A111" t="s">
+        <v>4</v>
+      </c>
+      <c r="B111" s="1">
+        <v>44000</v>
+      </c>
+      <c r="C111">
+        <v>49</v>
+      </c>
+      <c r="D111">
+        <f>SUM($C$2:C111)</f>
+        <v>28397</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A112" t="s">
+        <v>4</v>
+      </c>
+      <c r="B112" s="1">
+        <v>44001</v>
+      </c>
+      <c r="C112">
+        <v>42</v>
+      </c>
+      <c r="D112">
+        <f>SUM($C$2:C112)</f>
+        <v>28439</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A113" t="s">
+        <v>4</v>
+      </c>
+      <c r="B113" s="1">
+        <v>44002</v>
+      </c>
+      <c r="C113">
+        <v>45</v>
+      </c>
+      <c r="D113">
+        <f>SUM($C$2:C113)</f>
+        <v>28484</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A114" t="s">
+        <v>4</v>
+      </c>
+      <c r="B114" s="1">
+        <v>44003</v>
+      </c>
+      <c r="C114">
+        <v>36</v>
+      </c>
+      <c r="D114">
+        <f>SUM($C$2:C114)</f>
+        <v>28520</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A115" t="s">
+        <v>4</v>
+      </c>
+      <c r="B115" s="1">
+        <v>44004</v>
+      </c>
+      <c r="C115">
+        <v>42</v>
+      </c>
+      <c r="D115">
+        <f>SUM($C$2:C115)</f>
+        <v>28562</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A116" t="s">
+        <v>4</v>
+      </c>
+      <c r="B116" s="1">
+        <v>44005</v>
+      </c>
+      <c r="C116">
+        <v>51</v>
+      </c>
+      <c r="D116">
+        <f>SUM($C$2:C116)</f>
+        <v>28613</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A117" t="s">
+        <v>4</v>
+      </c>
+      <c r="B117" s="1">
+        <v>44006</v>
+      </c>
+      <c r="C117">
+        <v>54</v>
+      </c>
+      <c r="D117">
+        <f>SUM($C$2:C117)</f>
+        <v>28667</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A118" t="s">
+        <v>4</v>
+      </c>
+      <c r="B118" s="1">
+        <v>44007</v>
+      </c>
+      <c r="C118">
+        <v>46</v>
+      </c>
+      <c r="D118">
+        <f>SUM($C$2:C118)</f>
+        <v>28713</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A119" t="s">
+        <v>4</v>
+      </c>
+      <c r="B119" s="1">
+        <v>44008</v>
+      </c>
+      <c r="C119">
+        <v>36</v>
+      </c>
+      <c r="D119">
+        <f>SUM($C$2:C119)</f>
+        <v>28749</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A120" t="s">
+        <v>4</v>
+      </c>
+      <c r="B120" s="1">
+        <v>44009</v>
+      </c>
+      <c r="C120">
+        <v>30</v>
+      </c>
+      <c r="D120">
+        <f>SUM($C$2:C120)</f>
+        <v>28779</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A121" t="s">
+        <v>4</v>
+      </c>
+      <c r="B121" s="1">
+        <v>44010</v>
+      </c>
+      <c r="C121">
+        <v>37</v>
+      </c>
+      <c r="D121">
+        <f>SUM($C$2:C121)</f>
+        <v>28816</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A122" t="s">
+        <v>4</v>
+      </c>
+      <c r="B122" s="1">
+        <v>44011</v>
+      </c>
+      <c r="C122">
+        <v>29</v>
+      </c>
+      <c r="D122">
+        <f>SUM($C$2:C122)</f>
+        <v>28845</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A123" t="s">
+        <v>4</v>
+      </c>
+      <c r="B123" s="1">
+        <v>44012</v>
+      </c>
+      <c r="C123">
+        <v>29</v>
+      </c>
+      <c r="D123">
+        <f>SUM($C$2:C123)</f>
+        <v>28874</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A124" t="s">
+        <v>4</v>
+      </c>
+      <c r="B124" s="1">
+        <v>44013</v>
+      </c>
+      <c r="C124">
+        <v>17</v>
+      </c>
+      <c r="D124">
+        <f>SUM($C$2:C124)</f>
+        <v>28891</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A125" t="s">
+        <v>4</v>
+      </c>
+      <c r="B125" s="1">
+        <v>44014</v>
+      </c>
+      <c r="C125">
+        <v>33</v>
+      </c>
+      <c r="D125">
+        <f>SUM($C$2:C125)</f>
+        <v>28924</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A126" t="s">
+        <v>4</v>
+      </c>
+      <c r="B126" s="1">
+        <v>44015</v>
+      </c>
+      <c r="C126">
+        <v>18</v>
+      </c>
+      <c r="D126">
+        <f>SUM($C$2:C126)</f>
+        <v>28942</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A127" t="s">
+        <v>4</v>
+      </c>
+      <c r="B127" s="1">
+        <v>44016</v>
+      </c>
+      <c r="C127">
+        <v>21</v>
+      </c>
+      <c r="D127">
+        <f>SUM($C$2:C127)</f>
+        <v>28963</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A128" t="s">
+        <v>4</v>
+      </c>
+      <c r="B128" s="1">
+        <v>44017</v>
+      </c>
+      <c r="C128">
+        <v>23</v>
+      </c>
+      <c r="D128">
+        <f>SUM($C$2:C128)</f>
+        <v>28986</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A129" t="s">
+        <v>4</v>
+      </c>
+      <c r="B129" s="1">
+        <v>44018</v>
+      </c>
+      <c r="C129">
+        <v>23</v>
+      </c>
+      <c r="D129">
+        <f>SUM($C$2:C129)</f>
+        <v>29009</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A130" t="s">
+        <v>4</v>
+      </c>
+      <c r="B130" s="1">
+        <v>44019</v>
+      </c>
+      <c r="C130">
+        <v>22</v>
+      </c>
+      <c r="D130">
+        <f>SUM($C$2:C130)</f>
+        <v>29031</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A131" t="s">
+        <v>4</v>
+      </c>
+      <c r="B131" s="1">
+        <v>44020</v>
+      </c>
+      <c r="C131">
+        <v>21</v>
+      </c>
+      <c r="D131">
+        <f>SUM($C$2:C131)</f>
+        <v>29052</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A132" t="s">
+        <v>4</v>
+      </c>
+      <c r="B132" s="1">
+        <v>44021</v>
+      </c>
+      <c r="C132">
+        <v>37</v>
+      </c>
+      <c r="D132">
+        <f>SUM($C$2:C132)</f>
+        <v>29089</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A133" t="s">
+        <v>4</v>
+      </c>
+      <c r="B133" s="1">
+        <v>44022</v>
+      </c>
+      <c r="C133">
+        <v>16</v>
+      </c>
+      <c r="D133">
+        <f>SUM($C$2:C133)</f>
+        <v>29105</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A134" t="s">
+        <v>4</v>
+      </c>
+      <c r="B134" s="1">
+        <v>44023</v>
+      </c>
+      <c r="C134">
+        <v>9</v>
+      </c>
+      <c r="D134">
+        <f>SUM($C$2:C134)</f>
+        <v>29114</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A135" t="s">
+        <v>4</v>
+      </c>
+      <c r="B135" s="1">
+        <v>44024</v>
+      </c>
+      <c r="C135">
+        <v>14</v>
+      </c>
+      <c r="D135">
+        <f>SUM($C$2:C135)</f>
+        <v>29128</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A136" t="s">
+        <v>4</v>
+      </c>
+      <c r="B136" s="1">
+        <v>44025</v>
+      </c>
+      <c r="C136">
+        <v>21</v>
+      </c>
+      <c r="D136">
+        <f>SUM($C$2:C136)</f>
+        <v>29149</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A137" t="s">
+        <v>4</v>
+      </c>
+      <c r="B137" s="1">
+        <v>44026</v>
+      </c>
+      <c r="C137">
+        <v>10</v>
+      </c>
+      <c r="D137">
+        <f>SUM($C$2:C137)</f>
+        <v>29159</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A138" t="s">
+        <v>4</v>
+      </c>
+      <c r="B138" s="1">
+        <v>44027</v>
+      </c>
+      <c r="C138">
+        <v>17</v>
+      </c>
+      <c r="D138">
+        <f>SUM($C$2:C138)</f>
+        <v>29176</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A139" t="s">
+        <v>4</v>
+      </c>
+      <c r="B139" s="1">
+        <v>44028</v>
+      </c>
+      <c r="C139">
+        <v>8</v>
+      </c>
+      <c r="D139">
+        <f>SUM($C$2:C139)</f>
+        <v>29184</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A140" t="s">
+        <v>4</v>
+      </c>
+      <c r="B140" s="1">
+        <v>44029</v>
+      </c>
+      <c r="C140">
+        <v>6</v>
+      </c>
+      <c r="D140">
+        <f>SUM($C$2:C140)</f>
+        <v>29190</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A141" t="s">
+        <v>4</v>
+      </c>
+      <c r="B141" s="1">
+        <v>44030</v>
+      </c>
+      <c r="C141">
+        <v>10</v>
+      </c>
+      <c r="D141">
+        <f>SUM($C$2:C141)</f>
+        <v>29200</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A142" t="s">
+        <v>4</v>
+      </c>
+      <c r="B142" s="1">
+        <v>44031</v>
+      </c>
+      <c r="C142">
+        <v>4</v>
+      </c>
+      <c r="D142">
+        <f>SUM($C$2:C142)</f>
+        <v>29204</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A143" t="s">
+        <v>4</v>
+      </c>
+      <c r="B143" s="1">
+        <v>44032</v>
+      </c>
+      <c r="C143">
+        <v>0</v>
+      </c>
+      <c r="D143">
+        <f>SUM($C$2:C143)</f>
+        <v>29204</v>
       </c>
     </row>
   </sheetData>

</xml_diff>